<commit_message>
remove hourly earnings column
</commit_message>
<xml_diff>
--- a/datasets/employment/employment_stats_reformat.xlsx
+++ b/datasets/employment/employment_stats_reformat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wye\Documents\UIUC MCS\CS498\Create a narrative visualization\CS498NarrativeVisualization\datasets\employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AFC840-33AF-48A2-AFC5-4BAB3019FD0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F10375-C991-4F07-95F2-6347E221FD69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="900" windowWidth="24900" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="24900" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -225,21 +225,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="M126" authorId="0" shapeId="0" xr:uid="{966D4B3E-7F2A-4DC4-8AA0-0320DF990B0C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  preliminary
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B127" authorId="0" shapeId="0" xr:uid="{6AF9C186-6D70-4E2B-96A6-B2965E47FFCE}">
       <text>
         <r>
@@ -405,27 +390,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="M127" authorId="0" shapeId="0" xr:uid="{0F473C2A-5C54-494E-B040-E41D7837EADB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  preliminary
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>Jan-2010</t>
   </si>
@@ -836,9 +806,6 @@
   </si>
   <si>
     <t>Other services</t>
-  </si>
-  <si>
-    <t>Average hourly earnings of all employees, total private</t>
   </si>
   <si>
     <t>Total nonfarm</t>
@@ -848,9 +815,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0"/>
-    <numFmt numFmtId="165" formatCode="#0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -915,7 +881,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -933,9 +899,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1218,24 +1181,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M127"/>
+  <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="5" customWidth="1"/>
-    <col min="3" max="13" width="9.140625" style="3"/>
+    <col min="3" max="12" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>127</v>
@@ -1267,11 +1230,8 @@
       <c r="L1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1308,11 +1268,8 @@
       <c r="L2" s="6">
         <v>5323</v>
       </c>
-      <c r="M2" s="7">
-        <v>22.41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1349,11 +1306,8 @@
       <c r="L3" s="6">
         <v>5316</v>
       </c>
-      <c r="M3" s="7">
-        <v>22.45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1390,11 +1344,8 @@
       <c r="L4" s="6">
         <v>5329</v>
       </c>
-      <c r="M4" s="7">
-        <v>22.45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1431,11 +1382,8 @@
       <c r="L5" s="6">
         <v>5335</v>
       </c>
-      <c r="M5" s="7">
-        <v>22.49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1472,11 +1420,8 @@
       <c r="L6" s="6">
         <v>5330</v>
       </c>
-      <c r="M6" s="7">
-        <v>22.53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1513,11 +1458,8 @@
       <c r="L7" s="6">
         <v>5315</v>
       </c>
-      <c r="M7" s="7">
-        <v>22.53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1554,11 +1496,8 @@
       <c r="L8" s="6">
         <v>5326</v>
       </c>
-      <c r="M8" s="7">
-        <v>22.59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1595,11 +1534,8 @@
       <c r="L9" s="6">
         <v>5323</v>
       </c>
-      <c r="M9" s="7">
-        <v>22.62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1636,11 +1572,8 @@
       <c r="L10" s="6">
         <v>5332</v>
       </c>
-      <c r="M10" s="7">
-        <v>22.67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1677,11 +1610,8 @@
       <c r="L11" s="6">
         <v>5357</v>
       </c>
-      <c r="M11" s="7">
-        <v>22.74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1718,11 +1648,8 @@
       <c r="L12" s="6">
         <v>5346</v>
       </c>
-      <c r="M12" s="7">
-        <v>22.73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1759,11 +1686,8 @@
       <c r="L13" s="6">
         <v>5337</v>
       </c>
-      <c r="M13" s="7">
-        <v>22.76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1800,11 +1724,8 @@
       <c r="L14" s="6">
         <v>5327</v>
       </c>
-      <c r="M14" s="7">
-        <v>22.85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1841,11 +1762,8 @@
       <c r="L15" s="6">
         <v>5337</v>
       </c>
-      <c r="M15" s="7">
-        <v>22.87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1882,11 +1800,8 @@
       <c r="L16" s="6">
         <v>5333</v>
       </c>
-      <c r="M16" s="7">
-        <v>22.87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1923,11 +1838,8 @@
       <c r="L17" s="6">
         <v>5342</v>
       </c>
-      <c r="M17" s="7">
-        <v>22.92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1964,11 +1876,8 @@
       <c r="L18" s="6">
         <v>5346</v>
       </c>
-      <c r="M18" s="7">
-        <v>22.99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2005,11 +1914,8 @@
       <c r="L19" s="6">
         <v>5352</v>
       </c>
-      <c r="M19" s="7">
-        <v>23.01</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2046,11 +1952,8 @@
       <c r="L20" s="6">
         <v>5359</v>
       </c>
-      <c r="M20" s="7">
-        <v>23.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -2087,11 +1990,8 @@
       <c r="L21" s="6">
         <v>5376</v>
       </c>
-      <c r="M21" s="7">
-        <v>23.07</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -2128,11 +2028,8 @@
       <c r="L22" s="6">
         <v>5381</v>
       </c>
-      <c r="M22" s="7">
-        <v>23.11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -2169,11 +2066,8 @@
       <c r="L23" s="6">
         <v>5382</v>
       </c>
-      <c r="M23" s="7">
-        <v>23.21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -2210,11 +2104,8 @@
       <c r="L24" s="6">
         <v>5390</v>
       </c>
-      <c r="M24" s="7">
-        <v>23.18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -2251,11 +2142,8 @@
       <c r="L25" s="6">
         <v>5403</v>
       </c>
-      <c r="M25" s="7">
-        <v>23.21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -2292,11 +2180,8 @@
       <c r="L26" s="6">
         <v>5414</v>
       </c>
-      <c r="M26" s="7">
-        <v>23.24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -2333,11 +2218,8 @@
       <c r="L27" s="6">
         <v>5415</v>
       </c>
-      <c r="M27" s="7">
-        <v>23.27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -2374,11 +2256,8 @@
       <c r="L28" s="6">
         <v>5422</v>
       </c>
-      <c r="M28" s="7">
-        <v>23.36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -2415,11 +2294,8 @@
       <c r="L29" s="6">
         <v>5417</v>
       </c>
-      <c r="M29" s="7">
-        <v>23.39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -2456,11 +2332,8 @@
       <c r="L30" s="6">
         <v>5417</v>
       </c>
-      <c r="M30" s="7">
-        <v>23.39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -2497,11 +2370,8 @@
       <c r="L31" s="6">
         <v>5424</v>
       </c>
-      <c r="M31" s="7">
-        <v>23.46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2538,11 +2408,8 @@
       <c r="L32" s="6">
         <v>5433</v>
       </c>
-      <c r="M32" s="7">
-        <v>23.51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -2579,11 +2446,8 @@
       <c r="L33" s="6">
         <v>5431</v>
       </c>
-      <c r="M33" s="7">
-        <v>23.49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -2620,11 +2484,8 @@
       <c r="L34" s="6">
         <v>5442</v>
       </c>
-      <c r="M34" s="7">
-        <v>23.57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -2661,11 +2522,8 @@
       <c r="L35" s="6">
         <v>5446</v>
       </c>
-      <c r="M35" s="7">
-        <v>23.56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -2702,11 +2560,8 @@
       <c r="L36" s="6">
         <v>5449</v>
       </c>
-      <c r="M36" s="7">
-        <v>23.63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2743,11 +2598,8 @@
       <c r="L37" s="6">
         <v>5452</v>
       </c>
-      <c r="M37" s="7">
-        <v>23.73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -2784,11 +2636,8 @@
       <c r="L38" s="6">
         <v>5458</v>
       </c>
-      <c r="M38" s="7">
-        <v>23.76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -2825,11 +2674,8 @@
       <c r="L39" s="6">
         <v>5456</v>
       </c>
-      <c r="M39" s="7">
-        <v>23.77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -2866,11 +2712,8 @@
       <c r="L40" s="6">
         <v>5451</v>
       </c>
-      <c r="M40" s="7">
-        <v>23.81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -2907,11 +2750,8 @@
       <c r="L41" s="6">
         <v>5455</v>
       </c>
-      <c r="M41" s="7">
-        <v>23.87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -2948,11 +2788,8 @@
       <c r="L42" s="6">
         <v>5470</v>
       </c>
-      <c r="M42" s="7">
-        <v>23.89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -2989,11 +2826,8 @@
       <c r="L43" s="6">
         <v>5480</v>
       </c>
-      <c r="M43" s="7">
-        <v>23.97</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
@@ -3030,11 +2864,8 @@
       <c r="L44" s="6">
         <v>5483</v>
       </c>
-      <c r="M44" s="7">
-        <v>23.98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -3071,11 +2902,8 @@
       <c r="L45" s="6">
         <v>5494</v>
       </c>
-      <c r="M45" s="7">
-        <v>24.03</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -3112,11 +2940,8 @@
       <c r="L46" s="6">
         <v>5502</v>
       </c>
-      <c r="M46" s="7">
-        <v>24.06</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -3153,11 +2978,8 @@
       <c r="L47" s="6">
         <v>5509</v>
       </c>
-      <c r="M47" s="7">
-        <v>24.09</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -3194,11 +3016,8 @@
       <c r="L48" s="6">
         <v>5513</v>
       </c>
-      <c r="M48" s="7">
-        <v>24.16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
@@ -3235,11 +3054,8 @@
       <c r="L49" s="6">
         <v>5525</v>
       </c>
-      <c r="M49" s="7">
-        <v>24.17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
@@ -3276,11 +3092,8 @@
       <c r="L50" s="6">
         <v>5533</v>
       </c>
-      <c r="M50" s="7">
-        <v>24.21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
@@ -3317,11 +3130,8 @@
       <c r="L51" s="6">
         <v>5535</v>
       </c>
-      <c r="M51" s="7">
-        <v>24.32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
@@ -3358,11 +3168,8 @@
       <c r="L52" s="6">
         <v>5553</v>
       </c>
-      <c r="M52" s="7">
-        <v>24.31</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -3399,11 +3206,8 @@
       <c r="L53" s="6">
         <v>5565</v>
       </c>
-      <c r="M53" s="7">
-        <v>24.34</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -3440,11 +3244,8 @@
       <c r="L54" s="6">
         <v>5566</v>
       </c>
-      <c r="M54" s="7">
-        <v>24.4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -3481,11 +3282,8 @@
       <c r="L55" s="6">
         <v>5563</v>
       </c>
-      <c r="M55" s="7">
-        <v>24.44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -3522,11 +3320,8 @@
       <c r="L56" s="6">
         <v>5565</v>
       </c>
-      <c r="M56" s="7">
-        <v>24.48</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
@@ -3563,11 +3358,8 @@
       <c r="L57" s="6">
         <v>5580</v>
       </c>
-      <c r="M57" s="7">
-        <v>24.55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
@@ -3604,11 +3396,8 @@
       <c r="L58" s="6">
         <v>5575</v>
       </c>
-      <c r="M58" s="7">
-        <v>24.56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
@@ -3645,11 +3434,8 @@
       <c r="L59" s="6">
         <v>5582</v>
       </c>
-      <c r="M59" s="7">
-        <v>24.58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
@@ -3686,11 +3472,8 @@
       <c r="L60" s="6">
         <v>5590</v>
       </c>
-      <c r="M60" s="7">
-        <v>24.65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
@@ -3727,11 +3510,8 @@
       <c r="L61" s="6">
         <v>5592</v>
       </c>
-      <c r="M61" s="7">
-        <v>24.65</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
@@ -3768,11 +3548,8 @@
       <c r="L62" s="6">
         <v>5600</v>
       </c>
-      <c r="M62" s="7">
-        <v>24.73</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
@@ -3809,11 +3586,8 @@
       <c r="L63" s="6">
         <v>5605</v>
       </c>
-      <c r="M63" s="7">
-        <v>24.78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
@@ -3850,11 +3624,8 @@
       <c r="L64" s="6">
         <v>5607</v>
       </c>
-      <c r="M64" s="7">
-        <v>24.84</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
@@ -3891,11 +3662,8 @@
       <c r="L65" s="6">
         <v>5614</v>
       </c>
-      <c r="M65" s="7">
-        <v>24.89</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
@@ -3932,11 +3700,8 @@
       <c r="L66" s="6">
         <v>5623</v>
       </c>
-      <c r="M66" s="7">
-        <v>24.96</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>65</v>
       </c>
@@ -3973,11 +3738,8 @@
       <c r="L67" s="6">
         <v>5617</v>
       </c>
-      <c r="M67" s="7">
-        <v>24.98</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
@@ -4014,11 +3776,8 @@
       <c r="L68" s="6">
         <v>5629</v>
       </c>
-      <c r="M68" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>67</v>
       </c>
@@ -4055,11 +3814,8 @@
       <c r="L69" s="6">
         <v>5620</v>
       </c>
-      <c r="M69" s="7">
-        <v>25.1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>68</v>
       </c>
@@ -4096,11 +3852,8 @@
       <c r="L70" s="6">
         <v>5621</v>
       </c>
-      <c r="M70" s="7">
-        <v>25.11</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
@@ -4137,11 +3890,8 @@
       <c r="L71" s="6">
         <v>5630</v>
       </c>
-      <c r="M71" s="7">
-        <v>25.19</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
@@ -4178,11 +3928,8 @@
       <c r="L72" s="6">
         <v>5638</v>
       </c>
-      <c r="M72" s="7">
-        <v>25.24</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>71</v>
       </c>
@@ -4219,11 +3966,8 @@
       <c r="L73" s="6">
         <v>5653</v>
       </c>
-      <c r="M73" s="7">
-        <v>25.27</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>72</v>
       </c>
@@ -4260,11 +4004,8 @@
       <c r="L74" s="6">
         <v>5649</v>
       </c>
-      <c r="M74" s="7">
-        <v>25.36</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>73</v>
       </c>
@@ -4301,11 +4042,8 @@
       <c r="L75" s="6">
         <v>5666</v>
       </c>
-      <c r="M75" s="7">
-        <v>25.38</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>74</v>
       </c>
@@ -4342,11 +4080,8 @@
       <c r="L76" s="6">
         <v>5674</v>
       </c>
-      <c r="M76" s="7">
-        <v>25.45</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
@@ -4383,11 +4118,8 @@
       <c r="L77" s="6">
         <v>5678</v>
       </c>
-      <c r="M77" s="7">
-        <v>25.53</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
@@ -4424,11 +4156,8 @@
       <c r="L78" s="6">
         <v>5670</v>
       </c>
-      <c r="M78" s="7">
-        <v>25.58</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>77</v>
       </c>
@@ -4465,11 +4194,8 @@
       <c r="L79" s="6">
         <v>5681</v>
       </c>
-      <c r="M79" s="7">
-        <v>25.63</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
@@ -4506,11 +4232,8 @@
       <c r="L80" s="6">
         <v>5687</v>
       </c>
-      <c r="M80" s="7">
-        <v>25.7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>79</v>
       </c>
@@ -4547,11 +4270,8 @@
       <c r="L81" s="6">
         <v>5702</v>
       </c>
-      <c r="M81" s="7">
-        <v>25.72</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>80</v>
       </c>
@@ -4588,11 +4308,8 @@
       <c r="L82" s="6">
         <v>5713</v>
       </c>
-      <c r="M82" s="7">
-        <v>25.77</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>81</v>
       </c>
@@ -4629,11 +4346,8 @@
       <c r="L83" s="6">
         <v>5718</v>
       </c>
-      <c r="M83" s="7">
-        <v>25.88</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>82</v>
       </c>
@@ -4670,11 +4384,8 @@
       <c r="L84" s="6">
         <v>5729</v>
       </c>
-      <c r="M84" s="7">
-        <v>25.91</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
@@ -4711,11 +4422,8 @@
       <c r="L85" s="6">
         <v>5715</v>
       </c>
-      <c r="M85" s="7">
-        <v>25.94</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>84</v>
       </c>
@@ -4752,11 +4460,8 @@
       <c r="L86" s="6">
         <v>5731</v>
       </c>
-      <c r="M86" s="7">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
@@ -4793,11 +4498,8 @@
       <c r="L87" s="6">
         <v>5742</v>
       </c>
-      <c r="M87" s="7">
-        <v>26.08</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>86</v>
       </c>
@@ -4834,11 +4536,8 @@
       <c r="L88" s="6">
         <v>5745</v>
       </c>
-      <c r="M88" s="7">
-        <v>26.11</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
@@ -4875,11 +4574,8 @@
       <c r="L89" s="6">
         <v>5748</v>
       </c>
-      <c r="M89" s="7">
-        <v>26.17</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>88</v>
       </c>
@@ -4916,11 +4612,8 @@
       <c r="L90" s="6">
         <v>5759</v>
       </c>
-      <c r="M90" s="7">
-        <v>26.21</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>89</v>
       </c>
@@ -4957,11 +4650,8 @@
       <c r="L91" s="6">
         <v>5767</v>
       </c>
-      <c r="M91" s="7">
-        <v>26.27</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>90</v>
       </c>
@@ -4998,11 +4688,8 @@
       <c r="L92" s="6">
         <v>5774</v>
       </c>
-      <c r="M92" s="7">
-        <v>26.36</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
@@ -5039,11 +4726,8 @@
       <c r="L93" s="6">
         <v>5780</v>
       </c>
-      <c r="M93" s="7">
-        <v>26.38</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>92</v>
       </c>
@@ -5080,11 +4764,8 @@
       <c r="L94" s="6">
         <v>5773</v>
       </c>
-      <c r="M94" s="7">
-        <v>26.51</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>93</v>
       </c>
@@ -5121,11 +4802,8 @@
       <c r="L95" s="6">
         <v>5795</v>
       </c>
-      <c r="M95" s="7">
-        <v>26.48</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
@@ -5162,11 +4840,8 @@
       <c r="L96" s="6">
         <v>5806</v>
       </c>
-      <c r="M96" s="7">
-        <v>26.55</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>95</v>
       </c>
@@ -5203,11 +4878,8 @@
       <c r="L97" s="6">
         <v>5806</v>
       </c>
-      <c r="M97" s="7">
-        <v>26.64</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>96</v>
       </c>
@@ -5244,11 +4916,8 @@
       <c r="L98" s="6">
         <v>5811</v>
       </c>
-      <c r="M98" s="7">
-        <v>26.71</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>97</v>
       </c>
@@ -5285,11 +4954,8 @@
       <c r="L99" s="6">
         <v>5815</v>
       </c>
-      <c r="M99" s="7">
-        <v>26.75</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>98</v>
       </c>
@@ -5326,11 +4992,8 @@
       <c r="L100" s="6">
         <v>5812</v>
       </c>
-      <c r="M100" s="7">
-        <v>26.84</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>99</v>
       </c>
@@ -5367,11 +5030,8 @@
       <c r="L101" s="6">
         <v>5819</v>
       </c>
-      <c r="M101" s="7">
-        <v>26.91</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
@@ -5408,11 +5068,8 @@
       <c r="L102" s="6">
         <v>5831</v>
       </c>
-      <c r="M102" s="7">
-        <v>26.98</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>101</v>
       </c>
@@ -5449,11 +5106,8 @@
       <c r="L103" s="6">
         <v>5844</v>
       </c>
-      <c r="M103" s="7">
-        <v>27.04</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>102</v>
       </c>
@@ -5490,11 +5144,8 @@
       <c r="L104" s="6">
         <v>5829</v>
       </c>
-      <c r="M104" s="7">
-        <v>27.11</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>103</v>
       </c>
@@ -5531,11 +5182,8 @@
       <c r="L105" s="6">
         <v>5832</v>
       </c>
-      <c r="M105" s="7">
-        <v>27.22</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>104</v>
       </c>
@@ -5572,11 +5220,8 @@
       <c r="L106" s="6">
         <v>5837</v>
       </c>
-      <c r="M106" s="7">
-        <v>27.31</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>105</v>
       </c>
@@ -5613,11 +5258,8 @@
       <c r="L107" s="6">
         <v>5845</v>
       </c>
-      <c r="M107" s="7">
-        <v>27.36</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>106</v>
       </c>
@@ -5654,11 +5296,8 @@
       <c r="L108" s="6">
         <v>5842</v>
       </c>
-      <c r="M108" s="7">
-        <v>27.44</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>107</v>
       </c>
@@ -5695,11 +5334,8 @@
       <c r="L109" s="6">
         <v>5850</v>
       </c>
-      <c r="M109" s="7">
-        <v>27.54</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>108</v>
       </c>
@@ -5736,11 +5372,8 @@
       <c r="L110" s="6">
         <v>5853</v>
       </c>
-      <c r="M110" s="7">
-        <v>27.58</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>109</v>
       </c>
@@ -5777,11 +5410,8 @@
       <c r="L111" s="6">
         <v>5854</v>
       </c>
-      <c r="M111" s="7">
-        <v>27.69</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>110</v>
       </c>
@@ -5818,11 +5448,8 @@
       <c r="L112" s="6">
         <v>5869</v>
       </c>
-      <c r="M112" s="7">
-        <v>27.76</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>111</v>
       </c>
@@ -5859,11 +5486,8 @@
       <c r="L113" s="6">
         <v>5884</v>
       </c>
-      <c r="M113" s="7">
-        <v>27.81</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>112</v>
       </c>
@@ -5900,11 +5524,8 @@
       <c r="L114" s="6">
         <v>5881</v>
       </c>
-      <c r="M114" s="7">
-        <v>27.87</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>113</v>
       </c>
@@ -5941,11 +5562,8 @@
       <c r="L115" s="6">
         <v>5896</v>
       </c>
-      <c r="M115" s="7">
-        <v>27.96</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>114</v>
       </c>
@@ -5982,11 +5600,8 @@
       <c r="L116" s="6">
         <v>5905</v>
       </c>
-      <c r="M116" s="7">
-        <v>28.05</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>115</v>
       </c>
@@ -6023,11 +5638,8 @@
       <c r="L117" s="6">
         <v>5910</v>
       </c>
-      <c r="M117" s="7">
-        <v>28.16</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>116</v>
       </c>
@@ -6064,11 +5676,8 @@
       <c r="L118" s="6">
         <v>5907</v>
       </c>
-      <c r="M118" s="7">
-        <v>28.16</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>117</v>
       </c>
@@ -6105,11 +5714,8 @@
       <c r="L119" s="6">
         <v>5907</v>
       </c>
-      <c r="M119" s="7">
-        <v>28.24</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>118</v>
       </c>
@@ -6146,11 +5752,8 @@
       <c r="L120" s="6">
         <v>5923</v>
       </c>
-      <c r="M120" s="7">
-        <v>28.34</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>119</v>
       </c>
@@ -6187,11 +5790,8 @@
       <c r="L121" s="6">
         <v>5925</v>
       </c>
-      <c r="M121" s="7">
-        <v>28.37</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>120</v>
       </c>
@@ -6228,11 +5828,8 @@
       <c r="L122" s="6">
         <v>5935</v>
       </c>
-      <c r="M122" s="7">
-        <v>28.43</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>121</v>
       </c>
@@ -6269,11 +5866,8 @@
       <c r="L123" s="6">
         <v>5941</v>
       </c>
-      <c r="M123" s="7">
-        <v>28.52</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>122</v>
       </c>
@@ -6310,11 +5904,8 @@
       <c r="L124" s="6">
         <v>5850</v>
       </c>
-      <c r="M124" s="7">
-        <v>28.69</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>123</v>
       </c>
@@ -6351,11 +5942,8 @@
       <c r="L125" s="6">
         <v>4571</v>
       </c>
-      <c r="M125" s="7">
-        <v>30.03</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>124</v>
       </c>
@@ -6392,11 +5980,8 @@
       <c r="L126" s="6">
         <v>4832</v>
       </c>
-      <c r="M126" s="7">
-        <v>29.72</v>
-      </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>125</v>
       </c>
@@ -6432,9 +6017,6 @@
       </c>
       <c r="L127" s="6">
         <v>5189</v>
-      </c>
-      <c r="M127" s="7">
-        <v>29.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>